<commit_message>
changes to the treemap for publication
</commit_message>
<xml_diff>
--- a/data/raw/ind_nss2223_hdds.xlsx
+++ b/data/raw/ind_nss2223_hdds.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wfp-my.sharepoint.com/personal/gabriel_battcock_wfp_org/Documents/Documents/MIMI_mac/nsso_hces_2023/data/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wfp-my.sharepoint.com/personal/gabriel_battcock_wfp_org/Documents/Documents/MIMI_mac/git/india-lysine-wheat/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="8_{12FA55C3-B18D-4937-BABE-02992A857F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{801E79A6-E0AD-4BAF-B362-2E5B9C1A1BB0}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="8_{12FA55C3-B18D-4937-BABE-02992A857F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{429E2E22-8E70-46E3-AD39-789CE8C0D6B2}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{4B3BEF07-B5A6-47F0-8958-68537F84A5FE}"/>
+    <workbookView xWindow="28680" yWindow="945" windowWidth="29040" windowHeight="15720" xr2:uid="{4B3BEF07-B5A6-47F0-8958-68537F84A5FE}"/>
   </bookViews>
   <sheets>
     <sheet name="hdds" sheetId="1" r:id="rId1"/>
@@ -534,33 +534,12 @@
     <t>eggs</t>
   </si>
   <si>
-    <t>roots_tuber</t>
-  </si>
-  <si>
     <t>vegetables</t>
   </si>
   <si>
     <t>fruits</t>
   </si>
   <si>
-    <t>meat</t>
-  </si>
-  <si>
-    <t>fish</t>
-  </si>
-  <si>
-    <t>pulses_legumes_nuts</t>
-  </si>
-  <si>
-    <t>milk</t>
-  </si>
-  <si>
-    <t>oil</t>
-  </si>
-  <si>
-    <t>sugar</t>
-  </si>
-  <si>
     <t>misc</t>
   </si>
   <si>
@@ -589,6 +568,27 @@
   </si>
   <si>
     <t>meat_poultry_fish</t>
+  </si>
+  <si>
+    <t>roots and tubers</t>
+  </si>
+  <si>
+    <t>meat, poultry, offal</t>
+  </si>
+  <si>
+    <t>fish and seafood</t>
+  </si>
+  <si>
+    <t>pulses, legumes, nuts</t>
+  </si>
+  <si>
+    <t>milk and milk products</t>
+  </si>
+  <si>
+    <t>oil/fats</t>
+  </si>
+  <si>
+    <t>sugar/honey</t>
   </si>
 </sst>
 </file>
@@ -970,20 +970,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E9A87B2-4D66-40EF-B25E-B2D97F9AC5F9}">
   <dimension ref="A1:N163"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C138" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:N163"/>
+      <selection pane="bottomRight" activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.36328125" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -994,40 +994,40 @@
         <v>163</v>
       </c>
       <c r="D1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E1" t="s">
         <v>165</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>166</v>
       </c>
-      <c r="F1" t="s">
-        <v>167</v>
-      </c>
       <c r="G1" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="H1" t="s">
         <v>164</v>
       </c>
       <c r="I1" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="J1" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="K1" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="L1" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="M1" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="N1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>3</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>4</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>5</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>11</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>55</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>56</v>
       </c>
@@ -1093,7 +1093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>57</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>58</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>59</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>60</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>61</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>62</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>63</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>64</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>65</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>66</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>67</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>68</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>70</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>71</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>72</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>73</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>74</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>75</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>76</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>92</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>94</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>101</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>102</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>103</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>104</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>105</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>106</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>107</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>108</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>110</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>111</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>112</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>113</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>114</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>115</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>116</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>117</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>118</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>120</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>121</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>122</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>139</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>140</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>141</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>142</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>143</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>144</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>145</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>146</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>147</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>148</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>150</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>152</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>158</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>160</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>161</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>162</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>163</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>164</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>165</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>166</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>170</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>171</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>172</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>173</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>174</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>175</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>178</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>180</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>181</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>182</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>183</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>184</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>185</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>188</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>190</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>191</v>
       </c>
@@ -1937,7 +1937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>192</v>
       </c>
@@ -1948,7 +1948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>193</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>194</v>
       </c>
@@ -1970,7 +1970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>195</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>196</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>200</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>201</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>202</v>
       </c>
@@ -2022,7 +2022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>203</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>204</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>205</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>206</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>207</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>208</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>210</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>211</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>212</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>213</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>214</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>215</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>216</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>217</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>220</v>
       </c>
@@ -2187,7 +2187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>221</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>222</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>223</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>224</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>225</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>226</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>227</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>228</v>
       </c>
@@ -2275,7 +2275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>230</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>231</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>232</v>
       </c>
@@ -2308,7 +2308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>233</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>234</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>235</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>236</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>237</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>238</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>240</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>241</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>242</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>243</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>244</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>245</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>246</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>250</v>
       </c>
@@ -2462,7 +2462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>251</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>252</v>
       </c>
@@ -2484,7 +2484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>253</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>254</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>255</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>256</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>257</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>258</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>260</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>261</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A143" s="3">
         <v>263</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>270</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>271</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>272</v>
       </c>
@@ -2616,7 +2616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>273</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>274</v>
       </c>
@@ -2638,7 +2638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>275</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>276</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>278</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>280</v>
       </c>
@@ -2682,7 +2682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>281</v>
       </c>
@@ -2693,7 +2693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>282</v>
       </c>
@@ -2704,7 +2704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>283</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>284</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>290</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>291</v>
       </c>
@@ -2748,7 +2748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>292</v>
       </c>
@@ -2759,7 +2759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>293</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>294</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>295</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>296</v>
       </c>
@@ -2812,16 +2812,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1007B1C-E9C8-4A73-980F-04078FECD3B1}">
   <dimension ref="A1:M163"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1:D1048576"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2829,40 +2829,40 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F1" t="s">
         <v>175</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>176</v>
-      </c>
-      <c r="E1" t="s">
-        <v>177</v>
-      </c>
-      <c r="F1" t="s">
-        <v>182</v>
-      </c>
-      <c r="G1" t="s">
-        <v>183</v>
       </c>
       <c r="H1" t="s">
         <v>164</v>
       </c>
       <c r="I1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="J1" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="K1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="L1" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="M1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>3</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>4</v>
       </c>
@@ -2884,7 +2884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>5</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>11</v>
       </c>
@@ -2906,7 +2906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>55</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>56</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>57</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>58</v>
       </c>
@@ -2950,7 +2950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>59</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>60</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>61</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>62</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>63</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>64</v>
       </c>
@@ -3016,7 +3016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>65</v>
       </c>
@@ -3027,7 +3027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>66</v>
       </c>
@@ -3038,7 +3038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>67</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>68</v>
       </c>
@@ -3060,7 +3060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>70</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>71</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>72</v>
       </c>
@@ -3093,7 +3093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>73</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>74</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>75</v>
       </c>
@@ -3126,7 +3126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>76</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>92</v>
       </c>
@@ -3148,7 +3148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>94</v>
       </c>
@@ -3159,7 +3159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>101</v>
       </c>
@@ -3170,7 +3170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>102</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>103</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>104</v>
       </c>
@@ -3203,7 +3203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>105</v>
       </c>
@@ -3214,7 +3214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>106</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>107</v>
       </c>
@@ -3236,7 +3236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>108</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>110</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>111</v>
       </c>
@@ -3269,7 +3269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>112</v>
       </c>
@@ -3280,7 +3280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>113</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>114</v>
       </c>
@@ -3302,7 +3302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>115</v>
       </c>
@@ -3313,7 +3313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>116</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>117</v>
       </c>
@@ -3335,7 +3335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>118</v>
       </c>
@@ -3346,7 +3346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>120</v>
       </c>
@@ -3357,7 +3357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>121</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>122</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>139</v>
       </c>
@@ -3390,7 +3390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>140</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>141</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>142</v>
       </c>
@@ -3423,7 +3423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>143</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>144</v>
       </c>
@@ -3445,7 +3445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>145</v>
       </c>
@@ -3456,7 +3456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>146</v>
       </c>
@@ -3467,7 +3467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>147</v>
       </c>
@@ -3478,7 +3478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>148</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>150</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>152</v>
       </c>
@@ -3511,7 +3511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>158</v>
       </c>
@@ -3522,7 +3522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>160</v>
       </c>
@@ -3533,7 +3533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>161</v>
       </c>
@@ -3541,7 +3541,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>162</v>
       </c>
@@ -3552,7 +3552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>163</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>164</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>165</v>
       </c>
@@ -3585,7 +3585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>166</v>
       </c>
@@ -3596,7 +3596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>170</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>171</v>
       </c>
@@ -3618,7 +3618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>172</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>173</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>174</v>
       </c>
@@ -3651,7 +3651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>175</v>
       </c>
@@ -3662,7 +3662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>178</v>
       </c>
@@ -3673,7 +3673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>180</v>
       </c>
@@ -3684,7 +3684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>181</v>
       </c>
@@ -3695,7 +3695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>182</v>
       </c>
@@ -3706,7 +3706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>183</v>
       </c>
@@ -3717,7 +3717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>184</v>
       </c>
@@ -3728,7 +3728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>185</v>
       </c>
@@ -3739,7 +3739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>188</v>
       </c>
@@ -3750,7 +3750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>190</v>
       </c>
@@ -3761,7 +3761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>191</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>192</v>
       </c>
@@ -3783,7 +3783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>193</v>
       </c>
@@ -3794,7 +3794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>194</v>
       </c>
@@ -3805,7 +3805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>195</v>
       </c>
@@ -3816,7 +3816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>196</v>
       </c>
@@ -3827,7 +3827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>200</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>201</v>
       </c>
@@ -3846,7 +3846,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>202</v>
       </c>
@@ -3857,7 +3857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>203</v>
       </c>
@@ -3868,7 +3868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>204</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>205</v>
       </c>
@@ -3890,7 +3890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>206</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>207</v>
       </c>
@@ -3912,7 +3912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>208</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>210</v>
       </c>
@@ -3934,7 +3934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>211</v>
       </c>
@@ -3945,7 +3945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>212</v>
       </c>
@@ -3956,7 +3956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>213</v>
       </c>
@@ -3967,7 +3967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>214</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>215</v>
       </c>
@@ -3989,7 +3989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>216</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>217</v>
       </c>
@@ -4011,7 +4011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>220</v>
       </c>
@@ -4022,7 +4022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>221</v>
       </c>
@@ -4033,7 +4033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>222</v>
       </c>
@@ -4044,7 +4044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>223</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>224</v>
       </c>
@@ -4066,7 +4066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>225</v>
       </c>
@@ -4077,7 +4077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>226</v>
       </c>
@@ -4088,7 +4088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>227</v>
       </c>
@@ -4099,7 +4099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>228</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>230</v>
       </c>
@@ -4121,7 +4121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>231</v>
       </c>
@@ -4132,7 +4132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>232</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>233</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>234</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>235</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>236</v>
       </c>
@@ -4187,7 +4187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>237</v>
       </c>
@@ -4198,7 +4198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>238</v>
       </c>
@@ -4209,7 +4209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>240</v>
       </c>
@@ -4220,7 +4220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>241</v>
       </c>
@@ -4231,7 +4231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>242</v>
       </c>
@@ -4242,7 +4242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>243</v>
       </c>
@@ -4253,7 +4253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>244</v>
       </c>
@@ -4264,7 +4264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>245</v>
       </c>
@@ -4275,7 +4275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>246</v>
       </c>
@@ -4286,7 +4286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>250</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>251</v>
       </c>
@@ -4308,7 +4308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>252</v>
       </c>
@@ -4319,7 +4319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>253</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>254</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>255</v>
       </c>
@@ -4352,7 +4352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>256</v>
       </c>
@@ -4363,7 +4363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>257</v>
       </c>
@@ -4374,7 +4374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>258</v>
       </c>
@@ -4385,7 +4385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>260</v>
       </c>
@@ -4396,7 +4396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>261</v>
       </c>
@@ -4407,7 +4407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A143" s="3">
         <v>263</v>
       </c>
@@ -4418,7 +4418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>270</v>
       </c>
@@ -4429,7 +4429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>271</v>
       </c>
@@ -4440,7 +4440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>272</v>
       </c>
@@ -4451,7 +4451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>273</v>
       </c>
@@ -4462,7 +4462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>274</v>
       </c>
@@ -4473,7 +4473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>275</v>
       </c>
@@ -4484,7 +4484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>276</v>
       </c>
@@ -4495,7 +4495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>278</v>
       </c>
@@ -4506,7 +4506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>280</v>
       </c>
@@ -4517,7 +4517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>281</v>
       </c>
@@ -4528,7 +4528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>282</v>
       </c>
@@ -4539,7 +4539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>283</v>
       </c>
@@ -4550,7 +4550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>284</v>
       </c>
@@ -4561,7 +4561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>290</v>
       </c>
@@ -4572,7 +4572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>291</v>
       </c>
@@ -4583,7 +4583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>292</v>
       </c>
@@ -4594,7 +4594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>293</v>
       </c>
@@ -4605,7 +4605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>294</v>
       </c>
@@ -4616,7 +4616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>295</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>296</v>
       </c>

</xml_diff>